<commit_message>
O: get all accuracy data and update; upload accuracy.xlsx; done
</commit_message>
<xml_diff>
--- a/06_Result/Accuracy.xlsx
+++ b/06_Result/Accuracy.xlsx
@@ -424,18 +424,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -479,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -572,15 +566,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -597,6 +582,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -882,7 +873,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -936,10 +927,10 @@
       <c r="B3" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="32">
         <v>0.9002</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="35" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="5">
@@ -960,10 +951,10 @@
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="32">
         <v>0.98650000000000004</v>
       </c>
-      <c r="D4" s="39">
+      <c r="D4" s="36">
         <v>0.97989999999999999</v>
       </c>
       <c r="E4" s="5">
@@ -984,10 +975,10 @@
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="33">
         <v>0.13</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="37">
         <v>9.32</v>
       </c>
       <c r="E5" s="7">
@@ -1008,10 +999,10 @@
       <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="33">
         <v>0.24</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="37">
         <v>44.97</v>
       </c>
       <c r="E6" s="7">
@@ -1032,10 +1023,10 @@
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="33">
         <v>0.06</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="37">
         <v>-1.84</v>
       </c>
       <c r="E7" s="7">
@@ -1056,10 +1047,10 @@
       <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="33">
         <v>0.95</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="37">
         <v>0.94</v>
       </c>
       <c r="E8" s="7">
@@ -1082,11 +1073,11 @@
       <c r="B9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="34">
         <v>0.88429999999999997</v>
       </c>
-      <c r="D9" s="33">
-        <v>0.88160000000000005</v>
+      <c r="D9" s="39">
+        <v>0.92</v>
       </c>
       <c r="E9" s="10">
         <v>0.88949999999999996</v>
@@ -1106,11 +1097,11 @@
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="32">
-        <v>0.6</v>
-      </c>
-      <c r="D10" s="32">
-        <v>85.56</v>
+      <c r="C10" s="37">
+        <v>0.38</v>
+      </c>
+      <c r="D10" s="37">
+        <v>23.73</v>
       </c>
       <c r="E10" s="7">
         <v>0.32</v>
@@ -1130,11 +1121,11 @@
       <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="32">
-        <v>0.81</v>
-      </c>
-      <c r="D11" s="32">
-        <v>221.62</v>
+      <c r="C11" s="37">
+        <v>0.71</v>
+      </c>
+      <c r="D11" s="37">
+        <v>107.36</v>
       </c>
       <c r="E11" s="7">
         <v>0.6</v>
@@ -1154,11 +1145,11 @@
       <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="32">
-        <v>0.92</v>
-      </c>
-      <c r="D12" s="32">
-        <v>6.58</v>
+      <c r="C12" s="37">
+        <v>0.19</v>
+      </c>
+      <c r="D12" s="37">
+        <v>-2.0099999999999998</v>
       </c>
       <c r="E12" s="7">
         <v>0.15</v>
@@ -1178,11 +1169,11 @@
       <c r="B13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="34">
-        <v>0.77</v>
-      </c>
-      <c r="D13" s="34">
-        <v>0.81</v>
+      <c r="C13" s="38">
+        <v>0.85</v>
+      </c>
+      <c r="D13" s="38">
+        <v>0.84</v>
       </c>
       <c r="E13" s="13">
         <v>0.85</v>

</xml_diff>

<commit_message>
B: use new data to plot; revise the figure; done
</commit_message>
<xml_diff>
--- a/06_Result/Accuracy.xlsx
+++ b/06_Result/Accuracy.xlsx
@@ -539,24 +539,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -565,30 +589,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -873,7 +873,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -885,16 +885,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="30">
       <c r="A2" s="2"/>
@@ -921,16 +921,16 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="23">
         <v>0.9002</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="26" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="5">
@@ -947,14 +947,14 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="23"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="23">
         <v>0.98650000000000004</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="27">
         <v>0.97989999999999999</v>
       </c>
       <c r="E4" s="5">
@@ -971,14 +971,14 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="23"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="24">
         <v>0.13</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="28">
         <v>9.32</v>
       </c>
       <c r="E5" s="7">
@@ -995,14 +995,14 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="23"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="24">
         <v>0.24</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="28">
         <v>44.97</v>
       </c>
       <c r="E6" s="7">
@@ -1019,38 +1019,38 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="23"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="24">
         <v>0.06</v>
       </c>
-      <c r="D7" s="37">
-        <v>-1.84</v>
+      <c r="D7" s="28">
+        <v>-1.9</v>
       </c>
       <c r="E7" s="7">
         <v>0.05</v>
       </c>
       <c r="F7" s="7">
-        <v>-0.68</v>
+        <v>-0.74</v>
       </c>
       <c r="G7" s="7">
         <v>0.05</v>
       </c>
       <c r="H7" s="7">
-        <v>-0.77</v>
+        <v>-0.84</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="23"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="24">
         <v>0.95</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="28">
         <v>0.94</v>
       </c>
       <c r="E8" s="7">
@@ -1067,16 +1067,16 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="33" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="25">
         <v>0.88429999999999997</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="30">
         <v>0.92</v>
       </c>
       <c r="E9" s="10">
@@ -1093,14 +1093,14 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="25"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="28">
         <v>0.38</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="28">
         <v>23.73</v>
       </c>
       <c r="E10" s="7">
@@ -1117,14 +1117,14 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="25"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="28">
         <v>0.71</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="28">
         <v>107.36</v>
       </c>
       <c r="E11" s="7">
@@ -1141,38 +1141,38 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="25"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="28">
         <v>0.19</v>
       </c>
-      <c r="D12" s="37">
-        <v>-2.0099999999999998</v>
+      <c r="D12" s="28">
+        <v>-2.17</v>
       </c>
       <c r="E12" s="7">
         <v>0.15</v>
       </c>
       <c r="F12" s="7">
-        <v>-0.55000000000000004</v>
+        <v>-0.71</v>
       </c>
       <c r="G12" s="7">
         <v>0.15</v>
       </c>
       <c r="H12" s="7">
-        <v>-0.66</v>
+        <v>-0.81</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="26"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="29">
         <v>0.85</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="29">
         <v>0.84</v>
       </c>
       <c r="E13" s="13">
@@ -1189,7 +1189,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -1215,7 +1215,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="25"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
@@ -1239,7 +1239,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="25"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="8" t="s">
         <v>10</v>
       </c>
@@ -1263,7 +1263,7 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="25"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="8" t="s">
         <v>11</v>
       </c>
@@ -1287,7 +1287,7 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="26"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="12" t="s">
         <v>12</v>
       </c>
@@ -1311,7 +1311,7 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="33" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="9" t="s">
@@ -1337,7 +1337,7 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="25"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="4" t="s">
         <v>9</v>
       </c>
@@ -1361,7 +1361,7 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="25"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="8" t="s">
         <v>10</v>
       </c>
@@ -1385,7 +1385,7 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="25"/>
+      <c r="A22" s="34"/>
       <c r="B22" s="8" t="s">
         <v>11</v>
       </c>
@@ -1409,7 +1409,7 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="26"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="12" t="s">
         <v>12</v>
       </c>
@@ -1433,7 +1433,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -1459,7 +1459,7 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="25"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="4" t="s">
         <v>9</v>
       </c>
@@ -1483,7 +1483,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="25"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="8" t="s">
         <v>10</v>
       </c>
@@ -1507,7 +1507,7 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="25"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="8" t="s">
         <v>11</v>
       </c>
@@ -1531,7 +1531,7 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="26"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="12" t="s">
         <v>12</v>
       </c>
@@ -1555,7 +1555,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="33" t="s">
         <v>121</v>
       </c>
       <c r="B29" s="9" t="s">
@@ -1581,7 +1581,7 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="25"/>
+      <c r="A30" s="34"/>
       <c r="B30" s="4" t="s">
         <v>9</v>
       </c>
@@ -1605,7 +1605,7 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="25"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="8" t="s">
         <v>10</v>
       </c>
@@ -1629,7 +1629,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="25"/>
+      <c r="A32" s="34"/>
       <c r="B32" s="8" t="s">
         <v>11</v>
       </c>
@@ -1653,7 +1653,7 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="26"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="12" t="s">
         <v>12</v>
       </c>
@@ -1707,16 +1707,16 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1754,14 +1754,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -1784,7 +1784,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="75" customHeight="1">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="33" t="s">
         <v>76</v>
       </c>
       <c r="B3" s="17" t="s">
@@ -1793,42 +1793,42 @@
       <c r="C3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="33" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="25"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="18" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="26"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="19" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
     </row>
     <row r="6" spans="1:6" ht="45" customHeight="1">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="33" t="s">
         <v>77</v>
       </c>
       <c r="B6" s="17" t="s">
@@ -1837,363 +1837,363 @@
       <c r="C6" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="33" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="25"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="18" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:6" ht="30">
-      <c r="A8" s="25"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="20" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:6" ht="30">
-      <c r="A9" s="25"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="20" t="s">
         <v>40</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="1:6" ht="30">
-      <c r="A10" s="25"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="20" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
     </row>
     <row r="11" spans="1:6" ht="30">
-      <c r="A11" s="25"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="20" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:6" ht="30">
-      <c r="A12" s="25"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="20" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
     </row>
     <row r="13" spans="1:6" ht="30">
-      <c r="A13" s="25"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="20" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="25"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="20" t="s">
         <v>45</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="25"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="20" t="s">
         <v>46</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="25"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="20" t="s">
         <v>47</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:6" ht="30">
-      <c r="A17" s="25"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="20" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="25"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="20" t="s">
         <v>49</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="25"/>
+      <c r="A19" s="34"/>
       <c r="B19" s="20" t="s">
         <v>50</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="25"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="20" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="25"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="20" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="25"/>
+      <c r="A22" s="34"/>
       <c r="B22" s="20" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="25"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="20" t="s">
         <v>54</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="25"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="20" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="25"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="20" t="s">
         <v>56</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
     </row>
     <row r="26" spans="1:6" ht="30">
-      <c r="A26" s="25"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="20" t="s">
         <v>57</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
     </row>
     <row r="27" spans="1:6" ht="30">
-      <c r="A27" s="25"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="20" t="s">
         <v>58</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="25"/>
+      <c r="A28" s="34"/>
       <c r="B28" s="20" t="s">
         <v>59</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="25"/>
+      <c r="A29" s="34"/>
       <c r="B29" s="20" t="s">
         <v>60</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
     </row>
     <row r="30" spans="1:6" ht="30">
-      <c r="A30" s="25"/>
+      <c r="A30" s="34"/>
       <c r="B30" s="20" t="s">
         <v>61</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
     </row>
     <row r="31" spans="1:6" ht="30">
-      <c r="A31" s="25"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="20" t="s">
         <v>62</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
     </row>
     <row r="32" spans="1:6" ht="30">
-      <c r="A32" s="25"/>
+      <c r="A32" s="34"/>
       <c r="B32" s="20" t="s">
         <v>63</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
     </row>
     <row r="33" spans="1:6" ht="30">
-      <c r="A33" s="25"/>
+      <c r="A33" s="34"/>
       <c r="B33" s="20" t="s">
         <v>64</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
     </row>
     <row r="34" spans="1:6" ht="30">
-      <c r="A34" s="25"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="20" t="s">
         <v>65</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
     </row>
     <row r="35" spans="1:6" ht="30">
-      <c r="A35" s="26"/>
+      <c r="A35" s="35"/>
       <c r="B35" s="21" t="s">
         <v>66</v>
       </c>
       <c r="C35" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
@@ -2236,7 +2236,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="45">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="33" t="s">
         <v>75</v>
       </c>
       <c r="B38" s="17" t="s">
@@ -2245,54 +2245,54 @@
       <c r="C38" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="E38" s="24" t="s">
+      <c r="E38" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="24" t="s">
+      <c r="F38" s="33" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="60">
-      <c r="A39" s="25"/>
+      <c r="A39" s="34"/>
       <c r="B39" s="18" t="s">
         <v>79</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D39" s="30"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
     </row>
     <row r="40" spans="1:6" ht="45">
-      <c r="A40" s="25"/>
+      <c r="A40" s="34"/>
       <c r="B40" s="18" t="s">
         <v>82</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D40" s="30"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
     </row>
     <row r="41" spans="1:6" ht="60">
-      <c r="A41" s="25"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="18" t="s">
         <v>83</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D41" s="30"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
     </row>
     <row r="42" spans="1:6" ht="60">
-      <c r="A42" s="26"/>
+      <c r="A42" s="35"/>
       <c r="B42" s="19" t="s">
         <v>84</v>
       </c>
@@ -2310,7 +2310,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="45">
-      <c r="A43" s="24" t="s">
+      <c r="A43" s="33" t="s">
         <v>87</v>
       </c>
       <c r="B43" s="17" t="s">
@@ -2319,30 +2319,30 @@
       <c r="C43" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="D43" s="24" t="s">
+      <c r="D43" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="E43" s="24">
+      <c r="E43" s="33">
         <v>2015</v>
       </c>
-      <c r="F43" s="24" t="s">
+      <c r="F43" s="33" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="75">
-      <c r="A44" s="26"/>
+      <c r="A44" s="35"/>
       <c r="B44" s="19" t="s">
         <v>92</v>
       </c>
       <c r="C44" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
     </row>
     <row r="45" spans="1:6" ht="60">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="37" t="s">
         <v>94</v>
       </c>
       <c r="B45" s="22" t="s">
@@ -2362,7 +2362,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="60">
-      <c r="A46" s="30"/>
+      <c r="A46" s="38"/>
       <c r="B46" s="20" t="s">
         <v>96</v>
       </c>
@@ -2380,7 +2380,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="60">
-      <c r="A47" s="30"/>
+      <c r="A47" s="38"/>
       <c r="B47" s="20" t="s">
         <v>97</v>
       </c>
@@ -2398,7 +2398,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="60">
-      <c r="A48" s="30"/>
+      <c r="A48" s="38"/>
       <c r="B48" s="20" t="s">
         <v>98</v>
       </c>
@@ -2416,7 +2416,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="60">
-      <c r="A49" s="30"/>
+      <c r="A49" s="38"/>
       <c r="B49" s="20" t="s">
         <v>99</v>
       </c>
@@ -2434,109 +2434,109 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="60" customHeight="1">
-      <c r="A50" s="30"/>
+      <c r="A50" s="38"/>
       <c r="B50" s="20" t="s">
         <v>100</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D50" s="25" t="s">
+      <c r="D50" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="E50" s="25">
+      <c r="E50" s="34">
         <v>2006</v>
       </c>
-      <c r="F50" s="25" t="s">
+      <c r="F50" s="34" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="30">
-      <c r="A51" s="30"/>
+      <c r="A51" s="38"/>
       <c r="B51" s="20" t="s">
         <v>101</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="34"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="30"/>
+      <c r="A52" s="38"/>
       <c r="B52" s="20" t="s">
         <v>102</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="30"/>
+      <c r="A53" s="38"/>
       <c r="B53" s="20" t="s">
         <v>103</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="30"/>
+      <c r="A54" s="38"/>
       <c r="B54" s="20" t="s">
         <v>104</v>
       </c>
       <c r="C54" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="34"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="30"/>
+      <c r="A55" s="38"/>
       <c r="B55" s="20" t="s">
         <v>105</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="30"/>
+      <c r="A56" s="38"/>
       <c r="B56" s="20" t="s">
         <v>106</v>
       </c>
       <c r="C56" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="25"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
     </row>
     <row r="57" spans="1:6" ht="30">
-      <c r="A57" s="30"/>
+      <c r="A57" s="38"/>
       <c r="B57" s="20" t="s">
         <v>107</v>
       </c>
       <c r="C57" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="34"/>
     </row>
     <row r="58" spans="1:6" ht="60">
-      <c r="A58" s="31"/>
+      <c r="A58" s="39"/>
       <c r="B58" s="21" t="s">
         <v>108</v>
       </c>
@@ -2555,11 +2555,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="A6:A35"/>
-    <mergeCell ref="D6:D35"/>
-    <mergeCell ref="E6:E35"/>
-    <mergeCell ref="F6:F35"/>
     <mergeCell ref="D50:D57"/>
     <mergeCell ref="E50:E57"/>
     <mergeCell ref="F50:F57"/>
@@ -2576,6 +2571,11 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="F3:F5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="A6:A35"/>
+    <mergeCell ref="D6:D35"/>
+    <mergeCell ref="E6:E35"/>
+    <mergeCell ref="F6:F35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
C: revise; revise; done
</commit_message>
<xml_diff>
--- a/06_Result/Accuracy.xlsx
+++ b/06_Result/Accuracy.xlsx
@@ -873,7 +873,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -928,19 +928,19 @@
         <v>122</v>
       </c>
       <c r="C3" s="23">
-        <v>0.9002</v>
+        <v>0.90239999999999998</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="5">
-        <v>0.90449999999999997</v>
+        <v>0.90669999999999995</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="5">
-        <v>0.90410000000000001</v>
+        <v>0.90649999999999997</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>18</v>
@@ -952,22 +952,22 @@
         <v>0</v>
       </c>
       <c r="C4" s="23">
-        <v>0.98650000000000004</v>
+        <v>0.98680000000000001</v>
       </c>
       <c r="D4" s="27">
-        <v>0.97989999999999999</v>
+        <v>0.98629999999999995</v>
       </c>
       <c r="E4" s="5">
-        <v>0.98699999999999999</v>
+        <v>0.98729999999999996</v>
       </c>
       <c r="F4" s="5">
-        <v>0.98570000000000002</v>
+        <v>0.9859</v>
       </c>
       <c r="G4" s="5">
-        <v>0.98699999999999999</v>
+        <v>0.98729999999999996</v>
       </c>
       <c r="H4" s="5">
-        <v>0.98629999999999995</v>
+        <v>0.98670000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -979,19 +979,19 @@
         <v>0.13</v>
       </c>
       <c r="D5" s="28">
-        <v>9.32</v>
+        <v>9.1300000000000008</v>
       </c>
       <c r="E5" s="7">
         <v>0.11</v>
       </c>
       <c r="F5" s="7">
-        <v>4.4800000000000004</v>
+        <v>4.41</v>
       </c>
       <c r="G5" s="7">
         <v>0.11</v>
       </c>
       <c r="H5" s="7">
-        <v>4.7</v>
+        <v>4.59</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1003,19 +1003,19 @@
         <v>0.24</v>
       </c>
       <c r="D6" s="28">
-        <v>44.97</v>
+        <v>44.51</v>
       </c>
       <c r="E6" s="7">
         <v>0.2</v>
       </c>
       <c r="F6" s="7">
-        <v>22.25</v>
+        <v>22.14</v>
       </c>
       <c r="G6" s="7">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
       <c r="H6" s="7">
-        <v>22.75</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1027,19 +1027,19 @@
         <v>0.06</v>
       </c>
       <c r="D7" s="28">
-        <v>-1.9</v>
+        <v>-1.76</v>
       </c>
       <c r="E7" s="7">
         <v>0.05</v>
       </c>
       <c r="F7" s="7">
-        <v>-0.74</v>
+        <v>-0.67</v>
       </c>
       <c r="G7" s="7">
         <v>0.05</v>
       </c>
       <c r="H7" s="7">
-        <v>-0.84</v>
+        <v>-0.78</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1074,22 +1074,22 @@
         <v>0</v>
       </c>
       <c r="C9" s="25">
-        <v>0.88429999999999997</v>
+        <v>0.88670000000000004</v>
       </c>
       <c r="D9" s="30">
-        <v>0.92</v>
+        <v>0.92090000000000005</v>
       </c>
       <c r="E9" s="10">
-        <v>0.88949999999999996</v>
+        <v>0.89180000000000004</v>
       </c>
       <c r="F9" s="11">
-        <v>0.91900000000000004</v>
+        <v>0.91920000000000002</v>
       </c>
       <c r="G9" s="10">
-        <v>0.88900000000000001</v>
+        <v>0.89149999999999996</v>
       </c>
       <c r="H9" s="11">
-        <v>0.92</v>
+        <v>0.92159999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1101,19 +1101,19 @@
         <v>0.38</v>
       </c>
       <c r="D10" s="28">
-        <v>23.73</v>
+        <v>23.4</v>
       </c>
       <c r="E10" s="7">
         <v>0.32</v>
       </c>
       <c r="F10" s="7">
-        <v>11.57</v>
+        <v>11.43</v>
       </c>
       <c r="G10" s="7">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
       <c r="H10" s="7">
-        <v>12.13</v>
+        <v>11.91</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1122,22 +1122,22 @@
         <v>10</v>
       </c>
       <c r="C11" s="28">
-        <v>0.71</v>
+        <v>0.7</v>
       </c>
       <c r="D11" s="28">
-        <v>107.36</v>
+        <v>106.76</v>
       </c>
       <c r="E11" s="7">
         <v>0.6</v>
       </c>
       <c r="F11" s="7">
-        <v>52.87</v>
+        <v>52.8</v>
       </c>
       <c r="G11" s="7">
-        <v>0.61</v>
+        <v>0.6</v>
       </c>
       <c r="H11" s="7">
-        <v>55.01</v>
+        <v>54.44</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1149,19 +1149,19 @@
         <v>0.19</v>
       </c>
       <c r="D12" s="28">
-        <v>-2.17</v>
+        <v>-1.96</v>
       </c>
       <c r="E12" s="7">
         <v>0.15</v>
       </c>
       <c r="F12" s="7">
-        <v>-0.71</v>
+        <v>-0.59</v>
       </c>
       <c r="G12" s="7">
         <v>0.15</v>
       </c>
       <c r="H12" s="7">
-        <v>-0.81</v>
+        <v>-0.72</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1176,13 +1176,13 @@
         <v>0.84</v>
       </c>
       <c r="E13" s="13">
-        <v>0.85</v>
+        <v>0.86</v>
       </c>
       <c r="F13" s="13">
         <v>0.84</v>
       </c>
       <c r="G13" s="13">
-        <v>0.85</v>
+        <v>0.86</v>
       </c>
       <c r="H13" s="13">
         <v>0.84</v>
@@ -1196,22 +1196,22 @@
         <v>0</v>
       </c>
       <c r="C14" s="10">
-        <v>0.7651</v>
+        <v>0.76749999999999996</v>
       </c>
       <c r="D14" s="11">
-        <v>0.81899999999999995</v>
+        <v>0.82240000000000002</v>
       </c>
       <c r="E14" s="10">
-        <v>0.77569999999999995</v>
+        <v>0.77829999999999999</v>
       </c>
       <c r="F14" s="11">
-        <v>0.81589999999999996</v>
+        <v>0.81840000000000002</v>
       </c>
       <c r="G14" s="10">
-        <v>0.77339999999999998</v>
+        <v>0.77649999999999997</v>
       </c>
       <c r="H14" s="11">
-        <v>0.81620000000000004</v>
+        <v>0.81940000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1220,22 +1220,22 @@
         <v>9</v>
       </c>
       <c r="C15" s="7">
-        <v>0.62</v>
+        <v>0.61</v>
       </c>
       <c r="D15" s="7">
-        <v>36.19</v>
+        <v>35.81</v>
       </c>
       <c r="E15" s="7">
-        <v>0.52</v>
+        <v>0.51</v>
       </c>
       <c r="F15" s="7">
-        <v>17.760000000000002</v>
+        <v>17.61</v>
       </c>
       <c r="G15" s="7">
         <v>0.52</v>
       </c>
       <c r="H15" s="7">
-        <v>18.75</v>
+        <v>18.559999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1244,22 +1244,22 @@
         <v>10</v>
       </c>
       <c r="C16" s="7">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="D16" s="7">
-        <v>157.5</v>
+        <v>156</v>
       </c>
       <c r="E16" s="7">
         <v>0.86</v>
       </c>
       <c r="F16" s="7">
-        <v>78.28</v>
+        <v>77.760000000000005</v>
       </c>
       <c r="G16" s="7">
-        <v>0.88</v>
+        <v>0.87</v>
       </c>
       <c r="H16" s="7">
-        <v>80.86</v>
+        <v>80.16</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1268,22 +1268,22 @@
         <v>11</v>
       </c>
       <c r="C17" s="7">
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
       <c r="D17" s="7">
-        <v>2</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="E17" s="7">
-        <v>0.35</v>
+        <v>0.34</v>
       </c>
       <c r="F17" s="7">
-        <v>1.8</v>
+        <v>1.97</v>
       </c>
       <c r="G17" s="7">
         <v>0.35</v>
       </c>
       <c r="H17" s="7">
-        <v>1.65</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1295,19 +1295,19 @@
         <v>0.79</v>
       </c>
       <c r="D18" s="13">
-        <v>0.89</v>
+        <v>0.87</v>
       </c>
       <c r="E18" s="13">
         <v>0.81</v>
       </c>
       <c r="F18" s="13">
-        <v>0.89</v>
+        <v>0.88</v>
       </c>
       <c r="G18" s="13">
         <v>0.8</v>
       </c>
       <c r="H18" s="13">
-        <v>0.89</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1318,22 +1318,22 @@
         <v>0</v>
       </c>
       <c r="C19" s="10">
-        <v>0.9073</v>
+        <v>0.91010000000000002</v>
       </c>
       <c r="D19" s="11">
-        <v>0.8982</v>
+        <v>0.89970000000000006</v>
       </c>
       <c r="E19" s="10">
-        <v>0.91180000000000005</v>
+        <v>0.91449999999999998</v>
       </c>
       <c r="F19" s="11">
-        <v>0.89529999999999998</v>
+        <v>0.89610000000000001</v>
       </c>
       <c r="G19" s="10">
-        <v>0.91139999999999999</v>
+        <v>0.91420000000000001</v>
       </c>
       <c r="H19" s="11">
-        <v>0.90110000000000001</v>
+        <v>0.90249999999999997</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1342,22 +1342,22 @@
         <v>9</v>
       </c>
       <c r="C20" s="7">
-        <v>0.36</v>
+        <v>0.35</v>
       </c>
       <c r="D20" s="7">
-        <v>24.79</v>
+        <v>24.29</v>
       </c>
       <c r="E20" s="7">
-        <v>0.3</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F20" s="7">
-        <v>12.04</v>
+        <v>11.83</v>
       </c>
       <c r="G20" s="7">
         <v>0.3</v>
       </c>
       <c r="H20" s="7">
-        <v>12.55</v>
+        <v>12.29</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1366,22 +1366,22 @@
         <v>10</v>
       </c>
       <c r="C21" s="7">
-        <v>0.63</v>
+        <v>0.62</v>
       </c>
       <c r="D21" s="7">
-        <v>120.32</v>
+        <v>119.43</v>
       </c>
       <c r="E21" s="7">
         <v>0.53</v>
       </c>
       <c r="F21" s="7">
-        <v>59.86</v>
+        <v>59.63</v>
       </c>
       <c r="G21" s="7">
         <v>0.54</v>
       </c>
       <c r="H21" s="7">
-        <v>60.68</v>
+        <v>60.22</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1393,19 +1393,19 @@
         <v>0.16</v>
       </c>
       <c r="D22" s="7">
-        <v>-1.61</v>
+        <v>-1.39</v>
       </c>
       <c r="E22" s="7">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F22" s="7">
-        <v>-0.19</v>
+        <v>-0.06</v>
       </c>
       <c r="G22" s="7">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="H22" s="7">
-        <v>-0.2</v>
+        <v>-0.38</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1420,7 +1420,7 @@
         <v>0.78</v>
       </c>
       <c r="E23" s="13">
-        <v>0.85</v>
+        <v>0.86</v>
       </c>
       <c r="F23" s="13">
         <v>0.78</v>
@@ -1440,22 +1440,22 @@
         <v>0</v>
       </c>
       <c r="C24" s="10">
-        <v>0.93379999999999996</v>
+        <v>0.93610000000000004</v>
       </c>
       <c r="D24" s="11">
-        <v>0.95130000000000003</v>
+        <v>0.95279999999999998</v>
       </c>
       <c r="E24" s="10">
-        <v>0.93589999999999995</v>
+        <v>0.93810000000000004</v>
       </c>
       <c r="F24" s="11">
-        <v>0.95009999999999994</v>
+        <v>0.95079999999999998</v>
       </c>
       <c r="G24" s="10">
-        <v>0.93759999999999999</v>
+        <v>0.93989999999999996</v>
       </c>
       <c r="H24" s="11">
-        <v>0.95099999999999996</v>
+        <v>0.95320000000000005</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1464,22 +1464,22 @@
         <v>9</v>
       </c>
       <c r="C25" s="7">
-        <v>0.3</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D25" s="7">
-        <v>18.05</v>
+        <v>17.559999999999999</v>
       </c>
       <c r="E25" s="7">
         <v>0.25</v>
       </c>
       <c r="F25" s="7">
-        <v>8.86</v>
+        <v>8.68</v>
       </c>
       <c r="G25" s="7">
         <v>0.25</v>
       </c>
       <c r="H25" s="7">
-        <v>9.2200000000000006</v>
+        <v>8.94</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1488,22 +1488,22 @@
         <v>10</v>
       </c>
       <c r="C26" s="7">
-        <v>0.53</v>
+        <v>0.52</v>
       </c>
       <c r="D26" s="7">
-        <v>84.45</v>
+        <v>83.16</v>
       </c>
       <c r="E26" s="7">
-        <v>0.43</v>
+        <v>0.45</v>
       </c>
       <c r="F26" s="7">
-        <v>41.81</v>
+        <v>41.54</v>
       </c>
       <c r="G26" s="7">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="H26" s="7">
-        <v>43.41</v>
+        <v>42.42</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1515,19 +1515,19 @@
         <v>0.15</v>
       </c>
       <c r="D27" s="7">
-        <v>-2.36</v>
+        <v>-2.1</v>
       </c>
       <c r="E27" s="7">
         <v>0.12</v>
       </c>
       <c r="F27" s="7">
-        <v>-0.88</v>
+        <v>-0.73</v>
       </c>
       <c r="G27" s="7">
         <v>0.12</v>
       </c>
       <c r="H27" s="7">
-        <v>-0.9</v>
+        <v>-0.82</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1536,7 +1536,7 @@
         <v>12</v>
       </c>
       <c r="C28" s="13">
-        <v>0.88</v>
+        <v>0.89</v>
       </c>
       <c r="D28" s="13">
         <v>0.88</v>
@@ -1551,7 +1551,7 @@
         <v>0.89</v>
       </c>
       <c r="H28" s="13">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1">
@@ -1562,22 +1562,22 @@
         <v>0</v>
       </c>
       <c r="C29" s="10">
-        <v>0.92649999999999999</v>
+        <v>0.92920000000000003</v>
       </c>
       <c r="D29" s="11">
-        <v>0.83750000000000002</v>
+        <v>0.84870000000000001</v>
       </c>
       <c r="E29" s="11">
-        <v>0.92859999999999998</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="F29" s="11">
-        <v>0.84279999999999999</v>
+        <v>0.83320000000000005</v>
       </c>
       <c r="G29" s="10">
-        <v>0.93030000000000002</v>
+        <v>0.93310000000000004</v>
       </c>
       <c r="H29" s="11">
-        <v>0.8518</v>
+        <v>0.86109999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1586,22 +1586,22 @@
         <v>9</v>
       </c>
       <c r="C30" s="7">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="D30" s="7">
-        <v>24.02</v>
+        <v>23.21</v>
       </c>
       <c r="E30" s="7">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="F30" s="7">
-        <v>11.54</v>
+        <v>11.38</v>
       </c>
       <c r="G30" s="7">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="H30" s="7">
-        <v>11.99</v>
+        <v>11.59</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1610,22 +1610,22 @@
         <v>10</v>
       </c>
       <c r="C31" s="7">
-        <v>0.55000000000000004</v>
+        <v>0.54</v>
       </c>
       <c r="D31" s="7">
-        <v>157.18</v>
+        <v>151.69</v>
       </c>
       <c r="E31" s="7">
         <v>0.47</v>
       </c>
       <c r="F31" s="7">
-        <v>75.44</v>
+        <v>77.010000000000005</v>
       </c>
       <c r="G31" s="7">
-        <v>0.47</v>
+        <v>0.46</v>
       </c>
       <c r="H31" s="7">
-        <v>77.17</v>
+        <v>74.66</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1634,22 +1634,22 @@
         <v>11</v>
       </c>
       <c r="C32" s="7">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="D32" s="7">
-        <v>6.33</v>
+        <v>6.03</v>
       </c>
       <c r="E32" s="7">
         <v>0.15</v>
       </c>
       <c r="F32" s="7">
-        <v>3.39</v>
+        <v>3.61</v>
       </c>
       <c r="G32" s="7">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="H32" s="7">
-        <v>3.34</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1658,10 +1658,10 @@
         <v>12</v>
       </c>
       <c r="C33" s="13">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
       <c r="D33" s="13">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
       <c r="E33" s="13">
         <v>0.88</v>
@@ -1670,10 +1670,10 @@
         <v>0.7</v>
       </c>
       <c r="G33" s="13">
-        <v>0.88</v>
+        <v>0.89</v>
       </c>
       <c r="H33" s="13">
-        <v>0.71</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="1" customFormat="1">
@@ -1683,27 +1683,27 @@
       </c>
       <c r="C34" s="16">
         <f>(C14+C19+C29+C24)/4</f>
-        <v>0.88317500000000004</v>
+        <v>0.88572499999999998</v>
       </c>
       <c r="D34" s="16">
         <f t="shared" ref="D34:H34" si="0">(D14+D19+D29+D24)/4</f>
-        <v>0.87650000000000006</v>
+        <v>0.88090000000000002</v>
       </c>
       <c r="E34" s="16">
         <f t="shared" si="0"/>
-        <v>0.8879999999999999</v>
+        <v>0.89047500000000002</v>
       </c>
       <c r="F34" s="16">
         <f t="shared" si="0"/>
-        <v>0.87602499999999994</v>
+        <v>0.8746250000000001</v>
       </c>
       <c r="G34" s="16">
         <f t="shared" si="0"/>
-        <v>0.88817499999999994</v>
+        <v>0.89092499999999997</v>
       </c>
       <c r="H34" s="16">
         <f t="shared" si="0"/>
-        <v>0.88002500000000006</v>
+        <v>0.88405</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2555,6 +2555,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="A6:A35"/>
+    <mergeCell ref="D6:D35"/>
+    <mergeCell ref="E6:E35"/>
+    <mergeCell ref="F6:F35"/>
     <mergeCell ref="D50:D57"/>
     <mergeCell ref="E50:E57"/>
     <mergeCell ref="F50:F57"/>
@@ -2571,11 +2576,6 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="F3:F5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="A6:A35"/>
-    <mergeCell ref="D6:D35"/>
-    <mergeCell ref="E6:E35"/>
-    <mergeCell ref="F6:F35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>